<commit_message>
Smartphone as AR Tool - Registo
</commit_message>
<xml_diff>
--- a/00 - Recolha de Requisitos/RegistodePesquisas.xlsx
+++ b/00 - Recolha de Requisitos/RegistodePesquisas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FEBEC0-B44C-42C1-9A0C-D54ABB4E8A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FF1CAC-98B8-45A7-A258-946E63A6308F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -125,6 +125,35 @@
     <t>Keisuke Hattori
 Tatsunori Hirai</t>
   </si>
+  <si>
+    <t>Jinki Jung
+Jihye Hong
+Sungheon Park
+Hyun S. Yang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  A simulação demonstrou que este método interativo fornece uma forma fácil, acessível e conveniente a todos para manipular objetos virtuais, até mesmo pessoas sem qualquer experiência prévia.</t>
+  </si>
+  <si>
+    <t>C ++
+C#
+Java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smartphone
+Unity3D
+</t>
+  </si>
+  <si>
+    <t>Tornar a realidade aumentada acessível a qualquer pessoa a partir de um simples smartphone</t>
+  </si>
+  <si>
+    <t>Smartphone como ferramenta AR via Multi-Touch baseada no método de interações 3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smartphone as an augmented reality authoring tool via multi-touch based 3D interaction method | Proceedings of the 11th ACM SIGGRAPH International Conference on Virtual-Reality Continuum and its Applications in Industry
+</t>
+  </si>
 </sst>
 </file>
 
@@ -137,7 +166,7 @@
     <numFmt numFmtId="165" formatCode="#,##0_ ;\-#,##0\ "/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="49" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,6 +510,14 @@
       <color rgb="FF818B8A"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1" tint="0.14999847407452621"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="35">
@@ -842,7 +879,7 @@
     <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -955,40 +992,52 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="47" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="47" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1045,6 +1094,24 @@
   <dxfs count="20">
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA0C6CC"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="8" tint="0.59996337778862885"/>
+        </left>
+        <right style="thin">
+          <color theme="8" tint="0.59996337778862885"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1061,6 +1128,25 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1212,25 +1298,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1270,24 +1337,6 @@
         <scheme val="major"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA0C6CC"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="8" tint="0.59996337778862885"/>
-        </left>
-        <right style="thin">
-          <color theme="8" tint="0.59996337778862885"/>
-        </right>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1517,22 +1566,153 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>108859</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2567217</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1802279</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31BC9E78-0F50-9417-152E-801A58187A8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:srcRect b="2195"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4027716" y="4644572"/>
+          <a:ext cx="2458358" cy="1747850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>36285</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>44701</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2677263</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1950562</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DFCB3EA-7590-3F2B-7533-60BD7DCA03CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9588499" y="4634844"/>
+          <a:ext cx="2640978" cy="1905861"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3014890</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>707572</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5588267</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1514106</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{302758DD-D397-C66B-CC89-D763041C4324}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12567104" y="5297715"/>
+          <a:ext cx="2573377" cy="806534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TBL_Invitations" displayName="TBL_Convites" ref="A5:J16" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TBL_Invitations" displayName="TBL_Convites" ref="A5:J16" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Local/Contexto" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Objetivos" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Arquitetura global" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Dispositivos" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Tipos de Interação" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Packages de software" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Linguagens de programação" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Avaliação com peritos/utilizadores" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Public-domain" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Site" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Local/Contexto" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Objetivos" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Arquitetura global" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Dispositivos" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Tipos de Interação" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Packages de software" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Linguagens de programação" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Avaliação com peritos/utilizadores" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Public-domain" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Site" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2632,17 +2812,17 @@
   </sheetPr>
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="23.765625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.69140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.69140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="33.15234375" style="4" customWidth="1"/>
     <col min="4" max="4" width="35.07421875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="53.23046875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="70.921875" style="5" customWidth="1"/>
     <col min="6" max="7" width="23.69140625" style="5" customWidth="1"/>
     <col min="8" max="8" width="24.69140625" style="4" customWidth="1"/>
     <col min="9" max="10" width="23.69140625" style="4" customWidth="1"/>
@@ -2653,11 +2833,11 @@
   <sheetData>
     <row r="1" spans="1:16" ht="40.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="11"/>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="19"/>
@@ -2667,9 +2847,9 @@
       <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
       <c r="E2" s="24" t="s">
         <v>2</v>
       </c>
@@ -2683,12 +2863,12 @@
       <c r="P2" s="6"/>
     </row>
     <row r="3" spans="1:16" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
       <c r="E3" s="26">
         <f ca="1">TODAY()</f>
-        <v>44848</v>
+        <v>44850</v>
       </c>
       <c r="F3" s="35"/>
       <c r="G3" s="27"/>
@@ -2750,54 +2930,67 @@
       <c r="P5" s="6"/>
     </row>
     <row r="6" spans="1:16" s="1" customFormat="1" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="44" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="33"/>
-      <c r="H6" s="44" t="s">
+      <c r="H6" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="46" t="s">
+      <c r="I6" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="40" t="s">
+      <c r="J6" s="38" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="12"/>
+      <c r="L6" s="53"/>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="28"/>
-      <c r="B7" s="31"/>
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="163.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>26</v>
+      </c>
       <c r="C7" s="31"/>
-      <c r="D7" s="41"/>
+      <c r="D7" s="50" t="s">
+        <v>25</v>
+      </c>
       <c r="E7" s="32"/>
       <c r="F7" s="32"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33" t="s">
-        <v>1</v>
+      <c r="G7" s="49" t="s">
+        <v>24</v>
       </c>
-      <c r="I7" s="34"/>
-      <c r="J7" s="33"/>
+      <c r="H7" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="52" t="s">
+        <v>28</v>
+      </c>
       <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:16" ht="25.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="28"/>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
-      <c r="D8" s="42"/>
+      <c r="D8" s="39"/>
       <c r="E8" s="32"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
@@ -2818,7 +3011,7 @@
       <c r="H9" s="33"/>
       <c r="I9" s="34"/>
       <c r="J9" s="33"/>
-      <c r="K9" s="49"/>
+      <c r="K9" s="46"/>
       <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:16" ht="25.15" customHeight="1" x14ac:dyDescent="0.4">
@@ -3093,7 +3286,7 @@
     <mergeCell ref="B1:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="C13:C16 B11:B16">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3108,47 +3301,19 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="J6" r:id="rId1" xr:uid="{9C5F7A39-45A7-4854-A959-44BDC3812189}"/>
+    <hyperlink ref="J7" r:id="rId2" display="https://dl.acm.org/doi/abs/10.1145/2407516.2407520" xr:uid="{558B61DB-7002-4CE6-B6D2-EDC244EB1CC5}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <drawing r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3436,27 +3601,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141D71A4-5CC3-40CD-990C-070FB4B5F315}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D97E00F-6E84-416B-8452-E6DC935A7A92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44AF425-737A-413C-9CB5-588E99FE889D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3475,4 +3649,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D97E00F-6E84-416B-8452-E6DC935A7A92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141D71A4-5CC3-40CD-990C-070FB4B5F315}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Segurança no Trabalho - Brainstorm
</commit_message>
<xml_diff>
--- a/00 - Recolha de Requisitos/RegistodePesquisas.xlsx
+++ b/00 - Recolha de Requisitos/RegistodePesquisas.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F4BF7A-0BE4-4946-8D9C-3483B3908C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33ABD721-4ED6-4F9D-B765-BFEBDB96DB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brain Storming" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -371,6 +371,18 @@
   </si>
   <si>
     <t>Com base numa câmara e alguns sensores tem por objetivo, baseando-se em APIs desenvolvidas em liguagens acessiveis, fazer o tracking de movimentos e consequentemente mostrar os mesmos num ambiente virtualizado</t>
+  </si>
+  <si>
+    <t>Fábricas, Empresas</t>
+  </si>
+  <si>
+    <t>Tornar a tomada de conhecimento relativa à Segurança no Trabalho num processo interavtivo para boa compreensão dos trabalhadores</t>
+  </si>
+  <si>
+    <t>Obrigatoriamente todos os trabalhadores, especialmente de indústrias, devem tomar conhecimento e assinar um documento relativo à Segurança no Trabalho. No entanto poucos tomam atenção aos detalhes do documento, sendo um assunto bastante importante, devia existir algo mais interativo que levasse á compreensão total dos métodos a adotar para um trabalho seguro.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Através de uns óculos VR seria proporcionado um ambiente de trabalho virtual onde todas as regras de segurança e boas práticas no trabalho seriam demonstradas de forma simples e não ficassem na memória como tendo sido uma burocracia que os trabalhadores assinaram. </t>
   </si>
 </sst>
 </file>
@@ -1295,20 +1307,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -1902,14 +1914,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>5145318</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1788889</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1780271</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>11342</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>252640</xdr:rowOff>
     </xdr:to>
@@ -1940,8 +1952,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="8871860" y="-112485"/>
-          <a:ext cx="1809297" cy="2034268"/>
+          <a:off x="12344403" y="-341085"/>
+          <a:ext cx="1803854" cy="2486024"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3881,16 +3893,16 @@
   </sheetPr>
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="23.69140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.07421875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="70.921875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="23.69140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="63" style="5" customWidth="1"/>
+    <col min="4" max="4" width="51.69140625" style="5" customWidth="1"/>
     <col min="5" max="5" width="24.4609375" style="4" customWidth="1"/>
     <col min="6" max="6" width="1.4609375" style="5" customWidth="1"/>
     <col min="7" max="16384" width="10.69140625" style="5"/>
@@ -3898,14 +3910,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="11"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="61" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="59"/>
+      <c r="B2" s="62"/>
       <c r="C2" s="24" t="s">
         <v>1</v>
       </c>
@@ -3914,7 +3926,7 @@
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="59"/>
+      <c r="B3" s="62"/>
       <c r="C3" s="26">
         <f ca="1">TODAY()</f>
         <v>44853</v>
@@ -3946,10 +3958,18 @@
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" ht="159.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
+      <c r="A6" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>89</v>
+      </c>
       <c r="E6" s="47"/>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" ht="163.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -3957,6 +3977,7 @@
       <c r="B7" s="41"/>
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
+      <c r="E7" s="47"/>
     </row>
     <row r="8" spans="1:9" ht="162" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="41"/>
@@ -4162,7 +4183,7 @@
   </sheetPr>
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -4184,11 +4205,11 @@
   <sheetData>
     <row r="1" spans="1:16" ht="40.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="11"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="19"/>
@@ -4198,9 +4219,9 @@
       <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
       <c r="E2" s="24" t="s">
         <v>1</v>
       </c>
@@ -4214,9 +4235,9 @@
       <c r="P2" s="6"/>
     </row>
     <row r="3" spans="1:16" s="2" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="26">
         <f ca="1">TODAY()</f>
         <v>44853</v>
@@ -4280,7 +4301,7 @@
       <c r="L5" s="6"/>
       <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" s="1" customFormat="1" ht="159.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
         <v>19</v>
       </c>
@@ -4555,11 +4576,11 @@
       <c r="A15" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="61"/>
-      <c r="D15" s="62" t="s">
+      <c r="C15" s="59"/>
+      <c r="D15" s="60" t="s">
         <v>80</v>
       </c>
       <c r="E15" s="31"/>
@@ -4570,7 +4591,7 @@
       <c r="H15" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="I15" s="60" t="s">
+      <c r="I15" s="58" t="s">
         <v>82</v>
       </c>
       <c r="J15" s="35" t="s">
@@ -4778,6 +4799,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5065,36 +5115,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141D71A4-5CC3-40CD-990C-070FB4B5F315}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D97E00F-6E84-416B-8452-E6DC935A7A92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44AF425-737A-413C-9CB5-588E99FE889D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5113,24 +5154,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D97E00F-6E84-416B-8452-E6DC935A7A92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141D71A4-5CC3-40CD-990C-070FB4B5F315}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Instant Motion Tracking and Its Applications to Augmented Reality
</commit_message>
<xml_diff>
--- a/00 - Recolha de Requisitos/RegistodePesquisas.xlsx
+++ b/00 - Recolha de Requisitos/RegistodePesquisas.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355AE017-9F94-4BF1-8AE3-1721B147C21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA82902-56C9-410D-AD77-6E108AD55A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brain Storming" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="110">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -420,20 +420,51 @@
   <si>
     <t>indentificação de um objeto</t>
   </si>
+  <si>
+    <t>Sistema de rastreio de movimento sem calibragem, compativel com dispositivos acessíveis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A partir de uma imagem captada pelo Smartphone, em live é possivel, mesmo em casos de cenários estáticos:
+Inicializar uma projeção AR sem qualquer calibração prévia ou inicialização complexa;
+Desempenho em tempo real nos Smartphones, mostrando milhões de conteúdos de AR numa vasta gama de equipamentos acessiveis a inúmeros utilizadores
+</t>
+  </si>
+  <si>
+    <t>A arquitetura é composta por um módulo de análise de movimento, um outro para rastrear uma dada àrea ou de um alvo plano para superficies que devam ser projetadas num dado plano, caso não se trate de um contúdo onde este não seja necessário existe ainda um módulo de estimativa de pose para a calibração automática 6DoF.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smartphone
+VSlam
+</t>
+  </si>
+  <si>
+    <t>O sistema é capaz de reproduzir qualquer imagem 2D ou 3D num dado alvo, à escala pretendida sem qualquer tipo de Calibragem necessária, todos os testes realizados em smartphones tiveram resultados positivos.</t>
+  </si>
+  <si>
+    <t>Jianing Wei
+Genzhi Ye
+Tyler Mullen
+Matthias Grundmann
+Adel Ahmadyan
+Tingbo Hou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://research.google/pubs/pub48339/ </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="6">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="0000"/>
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0000"/>
   </numFmts>
-  <fonts count="53" x14ac:knownFonts="1">
+  <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -804,8 +835,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1003,6 +1041,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1122,11 +1166,11 @@
   </borders>
   <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1170,7 +1214,7 @@
     <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1268,7 +1312,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1319,7 +1363,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1352,85 +1396,91 @@
     <xf numFmtId="0" fontId="26" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="3" borderId="0" xfId="47" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="28" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="32" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="36" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="40" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="44" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="26" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="29" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="33" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="37" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="41" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="45" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="2" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="30" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="34" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="38" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="42" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="46" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="24" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="27" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="31" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="35" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="39" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="43" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="13" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="17" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Currency" xfId="4" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="22" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="12" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="8" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8"/>
-    <cellStyle name="Input" xfId="15" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="18" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="14" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Cor1" xfId="25" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Cor2" xfId="28" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Cor3" xfId="32" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Cor4" xfId="36" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Cor5" xfId="40" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Cor6" xfId="44" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Cor1" xfId="26" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Cor2" xfId="29" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Cor3" xfId="33" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Cor4" xfId="37" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Cor5" xfId="41" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Cor6" xfId="45" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Cor1" xfId="2" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Cor2" xfId="30" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Cor3" xfId="34" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Cor4" xfId="38" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Cor5" xfId="42" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Cor6" xfId="46" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 1" xfId="8" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="17" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula Ligada" xfId="18" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Cor1" xfId="24" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Cor2" xfId="27" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Cor3" xfId="31" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Cor4" xfId="35" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Cor5" xfId="39" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Cor6" xfId="43" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Correto" xfId="12" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="15" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hiperligação" xfId="47" builtinId="8"/>
+    <cellStyle name="Incorreto" xfId="13" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Moeda" xfId="4" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Moeda [0]" xfId="5" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="14" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="21" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="16" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="7" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Nota" xfId="21" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Percentagem" xfId="6" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Saída" xfId="16" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Separador de milhares [0]" xfId="3" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Texto de Aviso" xfId="20" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto Explicativo" xfId="22" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="7" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="23" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="20" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Verificar Célula" xfId="19" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="26">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA0C6CC"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="8" tint="0.59996337778862885"/>
-        </left>
-        <right style="thin">
-          <color theme="8" tint="0.59996337778862885"/>
-        </right>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1658,6 +1708,24 @@
         <scheme val="major"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA0C6CC"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="8" tint="0.59996337778862885"/>
+        </left>
+        <right style="thin">
+          <color theme="8" tint="0.59996337778862885"/>
+        </right>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2065,7 +2133,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1803400</xdr:colOff>
+      <xdr:colOff>1803399</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>459014</xdr:rowOff>
     </xdr:to>
@@ -2245,8 +2313,8 @@
       <xdr:rowOff>119744</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3140</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1590640</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>1937658</xdr:rowOff>
     </xdr:to>
@@ -2765,7 +2833,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>139004</xdr:colOff>
+      <xdr:colOff>139005</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>1999440</xdr:rowOff>
     </xdr:to>
@@ -2800,6 +2868,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028095</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>694999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4906226</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>4423342</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Imagem 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88666E59-979B-444D-B109-9A67DE6D9AAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11717262" y="25036666"/>
+          <a:ext cx="3878131" cy="3728343"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2821,18 +2933,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TBL_Invitations" displayName="TBL_Convites" ref="A5:J15" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TBL_Invitations" displayName="TBL_Convites" ref="A5:J15" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Local/Contexto" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Objetivos" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Arquitetura global" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Dispositivos" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Tipos de Interação" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Packages de software" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Linguagens de programação" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Avaliação com peritos/utilizadores" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Public-domain" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Site" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Local/Contexto" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Objetivos" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Arquitetura global" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Dispositivos" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Tipos de Interação" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Packages de software" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Linguagens de programação" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Avaliação com peritos/utilizadores" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Public-domain" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Site" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3932,31 +4044,31 @@
   </sheetPr>
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.08984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.69140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.07421875" style="1" customWidth="1"/>
     <col min="3" max="3" width="63" style="5" customWidth="1"/>
-    <col min="4" max="4" width="51.7265625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="24.453125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="1.453125" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="10.7265625" style="5"/>
+    <col min="4" max="4" width="51.69140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="24.4609375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="1.4609375" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="10.69140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="40.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="11"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="62" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="62"/>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="63"/>
       <c r="C2" s="24" t="s">
         <v>1</v>
       </c>
@@ -3964,23 +4076,23 @@
       <c r="E2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="62"/>
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="63"/>
       <c r="C3" s="26">
         <f ca="1">TODAY()</f>
-        <v>44853</v>
+        <v>44855</v>
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="15"/>
       <c r="C4" s="14"/>
       <c r="D4" s="21"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -3996,7 +4108,7 @@
       <c r="E5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="159.44999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="159.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="41" t="s">
         <v>87</v>
       </c>
@@ -4011,7 +4123,7 @@
       </c>
       <c r="E6" s="47"/>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="163.19999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="163.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="41" t="s">
         <v>91</v>
       </c>
@@ -4026,7 +4138,7 @@
       </c>
       <c r="E7" s="47"/>
     </row>
-    <row r="8" spans="1:9" ht="162" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="162" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="41" t="s">
         <v>92</v>
       </c>
@@ -4041,7 +4153,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="159.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="159.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="41" t="s">
         <v>98</v>
       </c>
@@ -4056,7 +4168,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="167.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="167.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="50" t="s">
         <v>102</v>
       </c>
@@ -4071,163 +4183,163 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="156.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="156.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="54"/>
       <c r="B11" s="54"/>
       <c r="C11" s="54"/>
       <c r="D11" s="54"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="25.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="28"/>
       <c r="B12" s="28"/>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="25.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="28"/>
       <c r="B13" s="28"/>
-      <c r="C13" s="63"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="28"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="25.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="28"/>
       <c r="B14" s="28"/>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="25.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="25.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="28"/>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="12"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
       <c r="D17" s="12"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="12"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
       <c r="D18" s="12"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="12"/>
       <c r="B20" s="13"/>
       <c r="C20" s="12"/>
       <c r="D20" s="20"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="10"/>
       <c r="D21" s="23"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="10"/>
       <c r="D22" s="9"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="47" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="49" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="50" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="51" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="52" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="53" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="54" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="55" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="57" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="59" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="64" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="65" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="66" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="67" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="68" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="69" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="70" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="71" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="72" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="73" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="74" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="75" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="76" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="77" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="78" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="79" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="80" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="81" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="82" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="83" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="29" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="30" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="31" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="32" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="33" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="34" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="35" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="37" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="38" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="39" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="40" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="41" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="42" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="43" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="44" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="45" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="46" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="47" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="48" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="49" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="50" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="51" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="52" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="53" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="54" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="55" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="56" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="57" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="58" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="59" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="60" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="61" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="62" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="63" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="64" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="65" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="66" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="67" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="68" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="69" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="70" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="71" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="72" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="73" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="74" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="75" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="76" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="77" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="78" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="79" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="80" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="81" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="82" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="83" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:B3"/>
@@ -4254,33 +4366,33 @@
   </sheetPr>
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="42" zoomScaleNormal="42" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="35.08984375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="70.90625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="50.26953125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="23.7265625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="24.7265625" style="4" customWidth="1"/>
-    <col min="9" max="10" width="23.7265625" style="4" customWidth="1"/>
-    <col min="11" max="12" width="24.453125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="1.453125" style="5" customWidth="1"/>
-    <col min="14" max="16384" width="10.7265625" style="5"/>
+    <col min="1" max="1" width="23.69140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.4609375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.15234375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="35.07421875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="70.921875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="50.23046875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="23.69140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="24.69140625" style="4" customWidth="1"/>
+    <col min="9" max="10" width="23.69140625" style="4" customWidth="1"/>
+    <col min="11" max="12" width="24.4609375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="1.4609375" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="10.69140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="40.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="11"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="19"/>
@@ -4289,10 +4401,10 @@
       <c r="J1" s="18"/>
       <c r="K1" s="12"/>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
+    <row r="2" spans="1:16" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="24" t="s">
         <v>1</v>
       </c>
@@ -4305,13 +4417,13 @@
       <c r="L2" s="6"/>
       <c r="P2" s="6"/>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
+    <row r="3" spans="1:16" s="2" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
       <c r="E3" s="26">
         <f ca="1">TODAY()</f>
-        <v>44853</v>
+        <v>44855</v>
       </c>
       <c r="F3" s="33"/>
       <c r="G3" s="27"/>
@@ -4322,7 +4434,7 @@
       <c r="L3" s="6"/>
       <c r="P3" s="6"/>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" s="2" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="15"/>
       <c r="C4" s="14"/>
       <c r="D4" s="34"/>
@@ -4337,7 +4449,7 @@
       <c r="K4" s="17"/>
       <c r="P4" s="6"/>
     </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" s="2" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -4372,7 +4484,7 @@
       <c r="L5" s="6"/>
       <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" ht="159.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="1" customFormat="1" ht="159.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
         <v>19</v>
       </c>
@@ -4404,7 +4516,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="47"/>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" ht="163.19999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="163.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="41" t="s">
         <v>26</v>
       </c>
@@ -4433,7 +4545,7 @@
       </c>
       <c r="K7" s="13"/>
     </row>
-    <row r="8" spans="1:16" ht="162" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="162" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="41" t="s">
         <v>28</v>
       </c>
@@ -4461,7 +4573,7 @@
       <c r="K8" s="13"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:16" ht="159.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="159.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="41" t="s">
         <v>38</v>
       </c>
@@ -4493,7 +4605,7 @@
       <c r="K9" s="42"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:16" ht="167.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="167.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="50" t="s">
         <v>41</v>
       </c>
@@ -4525,7 +4637,7 @@
       <c r="K10" s="13"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:16" ht="156.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="156.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="54" t="s">
         <v>48</v>
       </c>
@@ -4555,7 +4667,7 @@
       <c r="K11" s="13"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:16" ht="197.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="197.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="41" t="s">
         <v>55</v>
       </c>
@@ -4585,7 +4697,7 @@
       <c r="K12" s="13"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:16" ht="204.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="204.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="41" t="s">
         <v>66</v>
       </c>
@@ -4617,7 +4729,7 @@
       <c r="K13" s="13"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:16" ht="161.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" ht="161.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="41" t="s">
         <v>72</v>
       </c>
@@ -4649,7 +4761,7 @@
       <c r="K14" s="13"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:16" ht="184.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="185" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="57" t="s">
         <v>79</v>
       </c>
@@ -4677,21 +4789,34 @@
       <c r="K15" s="13"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="5"/>
+    <row r="16" spans="1:16" s="70" customFormat="1" ht="386.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="66" t="s">
+        <v>107</v>
+      </c>
+      <c r="I16" s="67" t="s">
+        <v>108</v>
+      </c>
+      <c r="J16" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="K16" s="69"/>
     </row>
-    <row r="17" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="12"/>
       <c r="B17" s="42"/>
       <c r="C17" s="13"/>
@@ -4705,7 +4830,7 @@
       <c r="K17" s="13"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -4719,7 +4844,7 @@
       <c r="K18" s="13"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -4733,7 +4858,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
@@ -4747,7 +4872,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -4761,87 +4886,87 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G22" s="4"/>
       <c r="J22" s="9"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G23" s="4"/>
       <c r="J23" s="9"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G24" s="4"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G25" s="4"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="47" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="49" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="50" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="51" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="52" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="53" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="54" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="55" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="57" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="59" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="64" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="65" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="66" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="67" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="68" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="69" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="70" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="71" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="72" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="73" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="74" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="75" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="76" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="77" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="78" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="79" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="80" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="81" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="82" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="29" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="30" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="31" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="32" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="33" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="34" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="35" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="37" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="38" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="39" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="40" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="41" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="42" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="43" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="44" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="45" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="46" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="47" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="48" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="49" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="50" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="51" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="52" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="53" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="54" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="55" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="56" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="57" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="58" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="59" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="60" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="61" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="62" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="63" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="64" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="65" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="66" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="67" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="68" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="69" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="70" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="71" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="72" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="73" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="74" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="75" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="76" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="77" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="78" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="79" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="80" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="81" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="82" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4864,18 +4989,48 @@
     <hyperlink ref="J13" r:id="rId7" xr:uid="{AA95B419-AF9B-4A3E-BE2B-A4C36838152B}"/>
     <hyperlink ref="J14" r:id="rId8" xr:uid="{01219542-9895-4F2E-9512-B6B5D3216204}"/>
     <hyperlink ref="J15" r:id="rId9" xr:uid="{1F3052D7-D354-4558-A0C3-60761279903A}"/>
+    <hyperlink ref="J16" r:id="rId10" xr:uid="{44BF53B1-C1BB-4504-B4FA-BB443EBBD225}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId10"/>
-  <drawing r:id="rId11"/>
+  <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId11"/>
+  <drawing r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5163,36 +5318,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141D71A4-5CC3-40CD-990C-070FB4B5F315}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D97E00F-6E84-416B-8452-E6DC935A7A92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44AF425-737A-413C-9CB5-588E99FE889D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5211,24 +5357,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D97E00F-6E84-416B-8452-E6DC935A7A92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{141D71A4-5CC3-40CD-990C-070FB4B5F315}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>